<commit_message>
added result unit selections (partially)
</commit_message>
<xml_diff>
--- a/Resources/Servopump motor and drive sizing KEB_V0.5_w_macros.xlsx
+++ b/Resources/Servopump motor and drive sizing KEB_V0.5_w_macros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kebautomation-my.sharepoint.com/personal/conner_glaser_kebamerica_com/Documents/Documents/PROJECTS/KEB/C/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kebautomation-my.sharepoint.com/personal/conner_glaser_kebamerica_com/Documents/Documents/PROJECTS/KEB/Product Calculator/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{6161D0D4-B3DF-42CE-8980-88386CA92AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B38E4FCA-9C4B-418C-A5D1-C1033D52FFC7}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="8_{6161D0D4-B3DF-42CE-8980-88386CA92AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4E3FB57-3407-4FF5-9AFC-7F05EE02A817}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="16080" windowWidth="20730" windowHeight="11760" tabRatio="581" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="4416" windowWidth="8856" windowHeight="4680" tabRatio="581" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="kgcm²_kgm²" comment="Convert inertia from: kgcm² to kgm²">1/10000</definedName>
     <definedName name="kgm²_kgcm²" comment="Convert inertia from: kgm² to kgcm²">10000</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5544,7 +5544,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6051,6 +6051,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6314,9 +6316,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -12974,8 +12973,8 @@
   </sheetPr>
   <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN21" sqref="AN21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -13023,41 +13022,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="303" t="s">
+      <c r="A1" s="305" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
       <c r="D1" s="195"/>
-      <c r="E1" s="295" t="s">
+      <c r="E1" s="297" t="s">
         <v>317</v>
       </c>
-      <c r="F1" s="295"/>
-      <c r="G1" s="296"/>
-      <c r="J1" s="307" t="s">
+      <c r="F1" s="297"/>
+      <c r="G1" s="298"/>
+      <c r="J1" s="309" t="s">
         <v>689</v>
       </c>
-      <c r="K1" s="307"/>
-      <c r="L1" s="307"/>
-      <c r="M1" s="307"/>
-      <c r="N1" s="307"/>
-      <c r="O1" s="307"/>
-      <c r="P1" s="307"/>
-      <c r="Q1" s="307"/>
-      <c r="S1" s="304" t="s">
+      <c r="K1" s="309"/>
+      <c r="L1" s="309"/>
+      <c r="M1" s="309"/>
+      <c r="N1" s="309"/>
+      <c r="O1" s="309"/>
+      <c r="P1" s="309"/>
+      <c r="Q1" s="309"/>
+      <c r="S1" s="306" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="305"/>
-      <c r="U1" s="305"/>
-      <c r="V1" s="305"/>
-      <c r="W1" s="305"/>
-      <c r="X1" s="305"/>
-      <c r="Y1" s="305"/>
-      <c r="Z1" s="305"/>
-      <c r="AA1" s="305"/>
-      <c r="AB1" s="305"/>
-      <c r="AC1" s="305"/>
-      <c r="AD1" s="306"/>
+      <c r="T1" s="307"/>
+      <c r="U1" s="307"/>
+      <c r="V1" s="307"/>
+      <c r="W1" s="307"/>
+      <c r="X1" s="307"/>
+      <c r="Y1" s="307"/>
+      <c r="Z1" s="307"/>
+      <c r="AA1" s="307"/>
+      <c r="AB1" s="307"/>
+      <c r="AC1" s="307"/>
+      <c r="AD1" s="308"/>
       <c r="AE1" s="247"/>
       <c r="AF1" s="247"/>
       <c r="AG1" s="247"/>
@@ -13065,7 +13064,7 @@
     </row>
     <row r="2" spans="1:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2"/>
-      <c r="H2" s="300" t="s">
+      <c r="H2" s="302" t="s">
         <v>648</v>
       </c>
       <c r="J2" s="248" t="s">
@@ -13087,7 +13086,7 @@
       </c>
     </row>
     <row r="3" spans="1:45" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="310" t="s">
+      <c r="A3" s="312" t="s">
         <v>315</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -13100,7 +13099,7 @@
         <f>SUM(E16)</f>
         <v>25.07</v>
       </c>
-      <c r="H3" s="301"/>
+      <c r="H3" s="303"/>
       <c r="J3" s="152" t="s">
         <v>692</v>
       </c>
@@ -13136,7 +13135,7 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="311"/>
+      <c r="A4" s="313"/>
       <c r="B4" s="12" t="s">
         <v>66</v>
       </c>
@@ -13146,7 +13145,7 @@
       <c r="E4" s="86">
         <v>110</v>
       </c>
-      <c r="H4" s="302"/>
+      <c r="H4" s="304"/>
       <c r="J4" s="251" t="s">
         <v>650</v>
       </c>
@@ -13173,7 +13172,7 @@
       </c>
     </row>
     <row r="5" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="311"/>
+      <c r="A5" s="313"/>
       <c r="B5" s="12" t="s">
         <v>68</v>
       </c>
@@ -13183,7 +13182,7 @@
       <c r="E5" s="85">
         <v>263.89999999999998</v>
       </c>
-      <c r="H5" s="300" t="s">
+      <c r="H5" s="302" t="s">
         <v>651</v>
       </c>
       <c r="J5" s="248" t="s">
@@ -13212,8 +13211,8 @@
       </c>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A6" s="311"/>
-      <c r="H6" s="301"/>
+      <c r="A6" s="313"/>
+      <c r="H6" s="303"/>
       <c r="J6" s="152" t="s">
         <v>654</v>
       </c>
@@ -13242,7 +13241,7 @@
       </c>
     </row>
     <row r="7" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="311"/>
+      <c r="A7" s="313"/>
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -13253,7 +13252,7 @@
         <f>E3*10000/E5/60</f>
         <v>15.83301755715549</v>
       </c>
-      <c r="H7" s="301"/>
+      <c r="H7" s="303"/>
       <c r="J7" s="152" t="s">
         <v>656</v>
       </c>
@@ -13282,7 +13281,7 @@
       </c>
     </row>
     <row r="8" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="311"/>
+      <c r="A8" s="313"/>
       <c r="B8" s="12" t="s">
         <v>316</v>
       </c>
@@ -13296,7 +13295,7 @@
         <f>ROUND(MAX(K22:K33),0)</f>
         <v>2533</v>
       </c>
-      <c r="H8" s="302"/>
+      <c r="H8" s="304"/>
       <c r="J8" s="152" t="s">
         <v>658</v>
       </c>
@@ -13306,7 +13305,7 @@
       <c r="Q8" s="153"/>
     </row>
     <row r="9" spans="1:45" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="312"/>
+      <c r="A9" s="314"/>
       <c r="B9" s="12" t="s">
         <v>468</v>
       </c>
@@ -13320,7 +13319,7 @@
         <f>E8/60/E9</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="H9" s="313" t="s">
+      <c r="H9" s="315" t="s">
         <v>659</v>
       </c>
       <c r="J9" s="248" t="s">
@@ -13344,7 +13343,7 @@
       </c>
     </row>
     <row r="10" spans="1:45" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H10" s="314"/>
+      <c r="H10" s="316"/>
       <c r="J10" s="152" t="s">
         <v>662</v>
       </c>
@@ -13367,21 +13366,21 @@
       </c>
     </row>
     <row r="11" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="310" t="s">
+      <c r="A11" s="312" t="s">
         <v>313</v>
       </c>
       <c r="B11" s="184" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="185"/>
-      <c r="E11" s="308" t="s">
+      <c r="E11" s="310" t="s">
         <v>480</v>
       </c>
-      <c r="F11" s="309"/>
+      <c r="F11" s="311"/>
       <c r="G11" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="H11" s="315"/>
+      <c r="H11" s="317"/>
       <c r="J11" s="251" t="s">
         <v>663</v>
       </c>
@@ -13416,7 +13415,7 @@
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A12" s="311"/>
+      <c r="A12" s="313"/>
       <c r="B12" s="12" t="s">
         <v>3</v>
       </c>
@@ -13447,7 +13446,7 @@
       </c>
     </row>
     <row r="13" spans="1:45" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="311"/>
+      <c r="A13" s="313"/>
       <c r="B13" s="12" t="s">
         <v>314</v>
       </c>
@@ -13461,7 +13460,7 @@
       <c r="H13" s="263"/>
     </row>
     <row r="14" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="311"/>
+      <c r="A14" s="313"/>
       <c r="B14" s="89" t="s">
         <v>312</v>
       </c>
@@ -13472,7 +13471,7 @@
         <f>VLOOKUP($E$11,HydraulicPumps[],11,FALSE)</f>
         <v>0.93</v>
       </c>
-      <c r="F14" s="297">
+      <c r="F14" s="299">
         <f>E14*E15</f>
         <v>0.85560000000000003</v>
       </c>
@@ -13488,7 +13487,7 @@
       </c>
     </row>
     <row r="15" spans="1:45" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A15" s="311"/>
+      <c r="A15" s="313"/>
       <c r="B15" s="89" t="s">
         <v>486</v>
       </c>
@@ -13499,7 +13498,7 @@
         <f>VLOOKUP($E$11,HydraulicPumps[],12,FALSE)</f>
         <v>0.92</v>
       </c>
-      <c r="F15" s="298"/>
+      <c r="F15" s="300"/>
       <c r="AM15" t="s">
         <v>680</v>
       </c>
@@ -13519,7 +13518,7 @@
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A16" s="312"/>
+      <c r="A16" s="314"/>
       <c r="B16" s="12" t="s">
         <v>69</v>
       </c>
@@ -13539,35 +13538,35 @@
       </c>
     </row>
     <row r="18" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E18" s="292" t="s">
+      <c r="E18" s="294" t="s">
         <v>546</v>
       </c>
-      <c r="F18" s="293"/>
+      <c r="F18" s="295"/>
       <c r="G18" s="159">
         <v>0.1</v>
       </c>
       <c r="H18" s="90"/>
-      <c r="J18" s="299" t="s">
+      <c r="J18" s="301" t="s">
         <v>77</v>
       </c>
-      <c r="K18" s="299"/>
-      <c r="L18" s="299"/>
-      <c r="M18" s="299"/>
-      <c r="N18" s="299"/>
-      <c r="O18" s="299"/>
-      <c r="P18" s="299"/>
-      <c r="Q18" s="299"/>
-      <c r="S18" s="294" t="s">
+      <c r="K18" s="301"/>
+      <c r="L18" s="301"/>
+      <c r="M18" s="301"/>
+      <c r="N18" s="301"/>
+      <c r="O18" s="301"/>
+      <c r="P18" s="301"/>
+      <c r="Q18" s="301"/>
+      <c r="S18" s="296" t="s">
         <v>469</v>
       </c>
-      <c r="T18" s="294"/>
-      <c r="U18" s="294"/>
-      <c r="V18" s="294"/>
-      <c r="W18" s="294"/>
-      <c r="X18" s="294"/>
-      <c r="Y18" s="294"/>
-      <c r="Z18" s="294"/>
-      <c r="AA18" s="294"/>
+      <c r="T18" s="296"/>
+      <c r="U18" s="296"/>
+      <c r="V18" s="296"/>
+      <c r="W18" s="296"/>
+      <c r="X18" s="296"/>
+      <c r="Y18" s="296"/>
+      <c r="Z18" s="296"/>
+      <c r="AA18" s="296"/>
       <c r="AM18" t="s">
         <v>680</v>
       </c>
@@ -13611,14 +13610,14 @@
       </c>
     </row>
     <row r="20" spans="1:42" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="B20" s="274" t="s">
+      <c r="B20" s="276" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="274"/>
-      <c r="D20" s="274"/>
-      <c r="E20" s="274"/>
-      <c r="F20" s="274"/>
-      <c r="G20" s="274"/>
+      <c r="C20" s="276"/>
+      <c r="D20" s="276"/>
+      <c r="E20" s="276"/>
+      <c r="F20" s="276"/>
+      <c r="G20" s="276"/>
       <c r="H20" s="186"/>
       <c r="J20" s="121" t="s">
         <v>72</v>
@@ -13732,7 +13731,7 @@
       </c>
     </row>
     <row r="22" spans="1:42" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="273" t="s">
+      <c r="A22" s="275" t="s">
         <v>310</v>
       </c>
       <c r="B22" s="258" t="s">
@@ -13814,7 +13813,7 @@
       </c>
     </row>
     <row r="23" spans="1:42" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="273"/>
+      <c r="A23" s="275"/>
       <c r="B23" s="118" t="s">
         <v>7</v>
       </c>
@@ -13901,7 +13900,7 @@
       </c>
     </row>
     <row r="24" spans="1:42" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="273"/>
+      <c r="A24" s="275"/>
       <c r="B24" s="118" t="s">
         <v>11</v>
       </c>
@@ -13988,7 +13987,7 @@
       </c>
     </row>
     <row r="25" spans="1:42" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="273"/>
+      <c r="A25" s="275"/>
       <c r="B25" s="118" t="s">
         <v>12</v>
       </c>
@@ -14075,7 +14074,7 @@
       </c>
     </row>
     <row r="26" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="273"/>
+      <c r="A26" s="275"/>
       <c r="B26" s="118" t="s">
         <v>13</v>
       </c>
@@ -14162,7 +14161,7 @@
       </c>
     </row>
     <row r="27" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="273"/>
+      <c r="A27" s="275"/>
       <c r="B27" s="118" t="s">
         <v>14</v>
       </c>
@@ -14239,7 +14238,7 @@
       </c>
     </row>
     <row r="28" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="273"/>
+      <c r="A28" s="275"/>
       <c r="B28" s="118" t="s">
         <v>622</v>
       </c>
@@ -14316,7 +14315,7 @@
       </c>
     </row>
     <row r="29" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="273"/>
+      <c r="A29" s="275"/>
       <c r="B29" s="118" t="s">
         <v>15</v>
       </c>
@@ -14393,7 +14392,7 @@
       </c>
     </row>
     <row r="30" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="273"/>
+      <c r="A30" s="275"/>
       <c r="B30" s="118" t="s">
         <v>16</v>
       </c>
@@ -14464,7 +14463,7 @@
       </c>
     </row>
     <row r="31" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="273"/>
+      <c r="A31" s="275"/>
       <c r="B31" s="118" t="s">
         <v>17</v>
       </c>
@@ -14535,7 +14534,7 @@
       </c>
     </row>
     <row r="32" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="273"/>
+      <c r="A32" s="275"/>
       <c r="B32" s="118" t="s">
         <v>18</v>
       </c>
@@ -14606,9 +14605,9 @@
       </c>
     </row>
     <row r="33" spans="1:40" ht="13.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="273"/>
-      <c r="B33" s="283"/>
-      <c r="C33" s="284"/>
+      <c r="A33" s="275"/>
+      <c r="B33" s="285"/>
+      <c r="C33" s="286"/>
       <c r="E33" s="12"/>
       <c r="F33" s="10"/>
       <c r="G33" s="6"/>
@@ -14675,10 +14674,10 @@
       </c>
     </row>
     <row r="34" spans="1:40" ht="3" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="283" t="s">
+      <c r="B34" s="285" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="284"/>
+      <c r="C34" s="286"/>
       <c r="E34" s="12">
         <v>0</v>
       </c>
@@ -14691,10 +14690,10 @@
       <c r="H34" s="186"/>
     </row>
     <row r="35" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="276" t="s">
+      <c r="B35" s="278" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="276"/>
+      <c r="C35" s="278"/>
       <c r="F35" s="165">
         <f>SUM(F22:F33)</f>
         <v>32.333333333333329</v>
@@ -14719,10 +14718,10 @@
       </c>
     </row>
     <row r="36" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="276" t="s">
+      <c r="B36" s="278" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="276"/>
+      <c r="C36" s="278"/>
       <c r="E36" s="161">
         <f>SQRT(SUMPRODUCT(E22:E33^2*F22:F33)/F35)</f>
         <v>57.988055114479323</v>
@@ -14779,10 +14778,10 @@
       </c>
     </row>
     <row r="38" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="277" t="s">
+      <c r="B38" s="279" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="277"/>
+      <c r="C38" s="279"/>
       <c r="E38" s="160">
         <f>MAX(E22:E33)</f>
         <v>181</v>
@@ -14881,38 +14880,38 @@
       <c r="B41"/>
     </row>
     <row r="42" spans="1:40" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="275" t="s">
+      <c r="B42" s="277" t="s">
         <v>548</v>
       </c>
-      <c r="C42" s="275"/>
-      <c r="D42" s="275"/>
-      <c r="E42" s="275"/>
-      <c r="F42" s="275"/>
-      <c r="G42" s="275"/>
-      <c r="J42" s="289" t="s">
+      <c r="C42" s="277"/>
+      <c r="D42" s="277"/>
+      <c r="E42" s="277"/>
+      <c r="F42" s="277"/>
+      <c r="G42" s="277"/>
+      <c r="J42" s="291" t="s">
         <v>176</v>
       </c>
-      <c r="K42" s="290"/>
-      <c r="L42" s="290"/>
-      <c r="M42" s="290"/>
-      <c r="N42" s="290"/>
-      <c r="O42" s="290"/>
-      <c r="P42" s="290"/>
-      <c r="Q42" s="290"/>
-      <c r="R42" s="290"/>
-      <c r="S42" s="291"/>
-      <c r="U42" s="288" t="s">
+      <c r="K42" s="292"/>
+      <c r="L42" s="292"/>
+      <c r="M42" s="292"/>
+      <c r="N42" s="292"/>
+      <c r="O42" s="292"/>
+      <c r="P42" s="292"/>
+      <c r="Q42" s="292"/>
+      <c r="R42" s="292"/>
+      <c r="S42" s="293"/>
+      <c r="U42" s="290" t="s">
         <v>198</v>
       </c>
-      <c r="V42" s="288"/>
-      <c r="W42" s="288"/>
-      <c r="X42" s="288"/>
-      <c r="Y42" s="288"/>
-      <c r="Z42" s="288"/>
-      <c r="AA42" s="288"/>
-      <c r="AB42" s="288"/>
-      <c r="AC42" s="288"/>
-      <c r="AD42" s="288"/>
+      <c r="V42" s="290"/>
+      <c r="W42" s="290"/>
+      <c r="X42" s="290"/>
+      <c r="Y42" s="290"/>
+      <c r="Z42" s="290"/>
+      <c r="AA42" s="290"/>
+      <c r="AB42" s="290"/>
+      <c r="AC42" s="290"/>
+      <c r="AD42" s="290"/>
     </row>
     <row r="43" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="18" t="s">
@@ -14925,7 +14924,7 @@
         <f>K36</f>
         <v>439.40115252168602</v>
       </c>
-      <c r="S43" s="286" t="s">
+      <c r="S43" s="288" t="s">
         <v>274</v>
       </c>
       <c r="AE43" s="3">
@@ -14936,13 +14935,13 @@
         <v>20</v>
       </c>
       <c r="AG43" s="59"/>
-      <c r="AH43" s="285" t="s">
+      <c r="AH43" s="287" t="s">
         <v>268</v>
       </c>
-      <c r="AI43" s="279" t="s">
+      <c r="AI43" s="281" t="s">
         <v>269</v>
       </c>
-      <c r="AJ43" s="279" t="s">
+      <c r="AJ43" s="281" t="s">
         <v>270</v>
       </c>
     </row>
@@ -14964,15 +14963,15 @@
       <c r="G44" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="J44" s="280" t="s">
+      <c r="J44" s="282" t="s">
         <v>549</v>
       </c>
-      <c r="K44" s="281"/>
-      <c r="L44" s="281"/>
-      <c r="M44" s="281"/>
-      <c r="N44" s="281"/>
-      <c r="O44" s="281"/>
-      <c r="P44" s="282"/>
+      <c r="K44" s="283"/>
+      <c r="L44" s="283"/>
+      <c r="M44" s="283"/>
+      <c r="N44" s="283"/>
+      <c r="O44" s="283"/>
+      <c r="P44" s="284"/>
       <c r="Q44" s="51">
         <f>$E$61/$E$66*380*1.25</f>
         <v>4418.9632715603248</v>
@@ -14980,13 +14979,13 @@
       <c r="R44" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="S44" s="287"/>
+      <c r="S44" s="289"/>
       <c r="AG44" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="AH44" s="285"/>
-      <c r="AI44" s="279"/>
-      <c r="AJ44" s="279"/>
+      <c r="AH44" s="287"/>
+      <c r="AI44" s="281"/>
+      <c r="AJ44" s="281"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B45" s="168" t="s">
@@ -14999,15 +14998,15 @@
         <f>MAX(P36,Z36)</f>
         <v>12.027906139667198</v>
       </c>
-      <c r="J45" s="280" t="s">
+      <c r="J45" s="282" t="s">
         <v>175</v>
       </c>
-      <c r="K45" s="281"/>
-      <c r="L45" s="281"/>
-      <c r="M45" s="281"/>
-      <c r="N45" s="281"/>
-      <c r="O45" s="281"/>
-      <c r="P45" s="282"/>
+      <c r="K45" s="283"/>
+      <c r="L45" s="283"/>
+      <c r="M45" s="283"/>
+      <c r="N45" s="283"/>
+      <c r="O45" s="283"/>
+      <c r="P45" s="284"/>
       <c r="Q45" s="6">
         <f>$E$58+($E$60-$E$58)/($E$61-100)*($E$43-100)</f>
         <v>21.356308159010595</v>
@@ -15019,16 +15018,16 @@
         <f>E45/Q45</f>
         <v>0.56320156321552317</v>
       </c>
-      <c r="U45" s="265" t="s">
+      <c r="U45" s="267" t="s">
         <v>233</v>
       </c>
-      <c r="V45" s="265"/>
-      <c r="W45" s="265"/>
-      <c r="X45" s="265"/>
-      <c r="Y45" s="265"/>
-      <c r="Z45" s="265"/>
-      <c r="AA45" s="265"/>
-      <c r="AB45" s="265"/>
+      <c r="V45" s="267"/>
+      <c r="W45" s="267"/>
+      <c r="X45" s="267"/>
+      <c r="Y45" s="267"/>
+      <c r="Z45" s="267"/>
+      <c r="AA45" s="267"/>
+      <c r="AB45" s="267"/>
       <c r="AC45" s="54">
         <f>E45/$E$65</f>
         <v>7.5067101328351891</v>
@@ -15061,15 +15060,15 @@
       <c r="G46" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="J46" s="280" t="s">
+      <c r="J46" s="282" t="s">
         <v>177</v>
       </c>
-      <c r="K46" s="281"/>
-      <c r="L46" s="281"/>
-      <c r="M46" s="281"/>
-      <c r="N46" s="281"/>
-      <c r="O46" s="281"/>
-      <c r="P46" s="282"/>
+      <c r="K46" s="283"/>
+      <c r="L46" s="283"/>
+      <c r="M46" s="283"/>
+      <c r="N46" s="283"/>
+      <c r="O46" s="283"/>
+      <c r="P46" s="284"/>
       <c r="Q46" s="6">
         <f>E62</f>
         <v>50</v>
@@ -15081,16 +15080,16 @@
         <f>E46/Q46</f>
         <v>0.77137061821861197</v>
       </c>
-      <c r="U46" s="265" t="s">
+      <c r="U46" s="267" t="s">
         <v>240</v>
       </c>
-      <c r="V46" s="265"/>
-      <c r="W46" s="265"/>
-      <c r="X46" s="265"/>
-      <c r="Y46" s="265"/>
-      <c r="Z46" s="265"/>
-      <c r="AA46" s="265"/>
-      <c r="AB46" s="265"/>
+      <c r="V46" s="267"/>
+      <c r="W46" s="267"/>
+      <c r="X46" s="267"/>
+      <c r="Y46" s="267"/>
+      <c r="Z46" s="267"/>
+      <c r="AA46" s="267"/>
+      <c r="AB46" s="267"/>
       <c r="AC46" s="6">
         <f>E46/$E$65</f>
         <v>24.070921275551356</v>
@@ -15144,14 +15143,14 @@
       <c r="O47" s="80"/>
       <c r="P47" s="80"/>
       <c r="R47" s="80"/>
-      <c r="W47" s="265" t="s">
+      <c r="W47" s="267" t="s">
         <v>199</v>
       </c>
-      <c r="X47" s="265"/>
-      <c r="Y47" s="265"/>
-      <c r="Z47" s="265"/>
-      <c r="AA47" s="265"/>
-      <c r="AB47" s="265"/>
+      <c r="X47" s="267"/>
+      <c r="Y47" s="267"/>
+      <c r="Z47" s="267"/>
+      <c r="AA47" s="267"/>
+      <c r="AB47" s="267"/>
       <c r="AC47" s="54">
         <f>AC46/1.5</f>
         <v>16.047280850367571</v>
@@ -15181,15 +15180,15 @@
       <c r="G48" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="J48" s="280" t="s">
+      <c r="J48" s="282" t="s">
         <v>271</v>
       </c>
-      <c r="K48" s="281"/>
-      <c r="L48" s="281"/>
-      <c r="M48" s="281"/>
-      <c r="N48" s="281"/>
-      <c r="O48" s="281"/>
-      <c r="P48" s="282"/>
+      <c r="K48" s="283"/>
+      <c r="L48" s="283"/>
+      <c r="M48" s="283"/>
+      <c r="N48" s="283"/>
+      <c r="O48" s="283"/>
+      <c r="P48" s="284"/>
       <c r="Q48" s="6">
         <f>$E$58+($E$60-$E$58)/($E$61-100)*($E$47-100)</f>
         <v>22.189655172413794</v>
@@ -15201,16 +15200,16 @@
         <f>E48/Q48</f>
         <v>0.32130055843930183</v>
       </c>
-      <c r="U48" s="265" t="s">
+      <c r="U48" s="267" t="s">
         <v>234</v>
       </c>
-      <c r="V48" s="265"/>
-      <c r="W48" s="265"/>
-      <c r="X48" s="265"/>
-      <c r="Y48" s="265"/>
-      <c r="Z48" s="265"/>
-      <c r="AA48" s="265"/>
-      <c r="AB48" s="265"/>
+      <c r="V48" s="267"/>
+      <c r="W48" s="267"/>
+      <c r="X48" s="267"/>
+      <c r="Y48" s="267"/>
+      <c r="Z48" s="267"/>
+      <c r="AA48" s="267"/>
+      <c r="AB48" s="267"/>
       <c r="AC48" s="6">
         <f>E48/$E$65</f>
         <v>4.449606946149002</v>
@@ -15286,15 +15285,15 @@
       <c r="G50" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="J50" s="280" t="s">
+      <c r="J50" s="282" t="s">
         <v>272</v>
       </c>
-      <c r="K50" s="281"/>
-      <c r="L50" s="281"/>
-      <c r="M50" s="281"/>
-      <c r="N50" s="281"/>
-      <c r="O50" s="281"/>
-      <c r="P50" s="282"/>
+      <c r="K50" s="283"/>
+      <c r="L50" s="283"/>
+      <c r="M50" s="283"/>
+      <c r="N50" s="283"/>
+      <c r="O50" s="283"/>
+      <c r="P50" s="284"/>
       <c r="Q50" s="6">
         <f>$E$58+($E$60-$E$58)/($E$61-100)*($E$49-100)</f>
         <v>22.189655172413794</v>
@@ -15306,16 +15305,16 @@
         <f>E50/Q50</f>
         <v>0.31870826417587367</v>
       </c>
-      <c r="U50" s="265" t="s">
+      <c r="U50" s="267" t="s">
         <v>235</v>
       </c>
-      <c r="V50" s="265"/>
-      <c r="W50" s="265"/>
-      <c r="X50" s="265"/>
-      <c r="Y50" s="265"/>
-      <c r="Z50" s="265"/>
-      <c r="AA50" s="265"/>
-      <c r="AB50" s="265"/>
+      <c r="V50" s="267"/>
+      <c r="W50" s="267"/>
+      <c r="X50" s="267"/>
+      <c r="Y50" s="267"/>
+      <c r="Z50" s="267"/>
+      <c r="AA50" s="267"/>
+      <c r="AB50" s="267"/>
       <c r="AC50" s="6">
         <f>E50/$E$65</f>
         <v>4.4137069445522377</v>
@@ -15391,15 +15390,15 @@
       <c r="G52" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="J52" s="280" t="s">
+      <c r="J52" s="282" t="s">
         <v>273</v>
       </c>
-      <c r="K52" s="281"/>
-      <c r="L52" s="281"/>
-      <c r="M52" s="281"/>
-      <c r="N52" s="281"/>
-      <c r="O52" s="281"/>
-      <c r="P52" s="282"/>
+      <c r="K52" s="283"/>
+      <c r="L52" s="283"/>
+      <c r="M52" s="283"/>
+      <c r="N52" s="283"/>
+      <c r="O52" s="283"/>
+      <c r="P52" s="284"/>
       <c r="Q52" s="6">
         <f>$E$58+($E$60-$E$58)/($E$61-100)*($E$52-100)</f>
         <v>22.189655172413794</v>
@@ -15411,16 +15410,16 @@
         <f>E52/Q52</f>
         <v>0</v>
       </c>
-      <c r="U52" s="265" t="s">
+      <c r="U52" s="267" t="s">
         <v>236</v>
       </c>
-      <c r="V52" s="265"/>
-      <c r="W52" s="265"/>
-      <c r="X52" s="265"/>
-      <c r="Y52" s="265"/>
-      <c r="Z52" s="265"/>
-      <c r="AA52" s="265"/>
-      <c r="AB52" s="265"/>
+      <c r="V52" s="267"/>
+      <c r="W52" s="267"/>
+      <c r="X52" s="267"/>
+      <c r="Y52" s="267"/>
+      <c r="Z52" s="267"/>
+      <c r="AA52" s="267"/>
+      <c r="AB52" s="267"/>
       <c r="AC52" s="6">
         <f>E52/$E$65</f>
         <v>0</v>
@@ -15463,15 +15462,15 @@
         <f>AA36</f>
         <v>0.81110792213508565</v>
       </c>
-      <c r="J53" s="280" t="s">
+      <c r="J53" s="282" t="s">
         <v>178</v>
       </c>
-      <c r="K53" s="281"/>
-      <c r="L53" s="281"/>
-      <c r="M53" s="281"/>
-      <c r="N53" s="281"/>
-      <c r="O53" s="281"/>
-      <c r="P53" s="282"/>
+      <c r="K53" s="283"/>
+      <c r="L53" s="283"/>
+      <c r="M53" s="283"/>
+      <c r="N53" s="283"/>
+      <c r="O53" s="283"/>
+      <c r="P53" s="284"/>
       <c r="Q53" s="6">
         <f>E59</f>
         <v>5.1836278784231586</v>
@@ -15501,28 +15500,28 @@
       <c r="B56" s="182" t="s">
         <v>157</v>
       </c>
-      <c r="C56" s="266" t="s">
+      <c r="C56" s="268" t="s">
         <v>438</v>
       </c>
-      <c r="D56" s="267"/>
-      <c r="E56" s="267"/>
-      <c r="F56" s="268"/>
+      <c r="D56" s="269"/>
+      <c r="E56" s="269"/>
+      <c r="F56" s="270"/>
       <c r="G56" s="60" t="s">
         <v>237</v>
       </c>
-      <c r="U56" s="270" t="s">
+      <c r="U56" s="272" t="s">
         <v>221</v>
       </c>
-      <c r="V56" s="271"/>
-      <c r="W56" s="271"/>
-      <c r="X56" s="271"/>
-      <c r="Y56" s="272"/>
-      <c r="Z56" s="267" t="s">
+      <c r="V56" s="273"/>
+      <c r="W56" s="273"/>
+      <c r="X56" s="273"/>
+      <c r="Y56" s="274"/>
+      <c r="Z56" s="269" t="s">
         <v>47</v>
       </c>
-      <c r="AA56" s="267"/>
-      <c r="AB56" s="267"/>
-      <c r="AC56" s="268"/>
+      <c r="AA56" s="269"/>
+      <c r="AB56" s="269"/>
+      <c r="AC56" s="270"/>
       <c r="AD56" s="60" t="s">
         <v>238</v>
       </c>
@@ -15552,15 +15551,15 @@
         <v>22</v>
       </c>
       <c r="F58" s="153"/>
-      <c r="U58" s="269" t="s">
+      <c r="U58" s="271" t="s">
         <v>230</v>
       </c>
-      <c r="V58" s="269"/>
-      <c r="W58" s="269"/>
-      <c r="X58" s="269"/>
-      <c r="Y58" s="269"/>
-      <c r="Z58" s="269"/>
-      <c r="AA58" s="269"/>
+      <c r="V58" s="271"/>
+      <c r="W58" s="271"/>
+      <c r="X58" s="271"/>
+      <c r="Y58" s="271"/>
+      <c r="Z58" s="271"/>
+      <c r="AA58" s="271"/>
       <c r="AB58" s="12">
         <f>VLOOKUP($Z$56,KEBDriveData[],3,FALSE)</f>
         <v>11</v>
@@ -15583,15 +15582,15 @@
         <v>5.1836278784231586</v>
       </c>
       <c r="F59" s="153"/>
-      <c r="U59" s="269" t="s">
+      <c r="U59" s="271" t="s">
         <v>232</v>
       </c>
-      <c r="V59" s="269"/>
-      <c r="W59" s="269"/>
-      <c r="X59" s="269"/>
-      <c r="Y59" s="269"/>
-      <c r="Z59" s="269"/>
-      <c r="AA59" s="269"/>
+      <c r="V59" s="271"/>
+      <c r="W59" s="271"/>
+      <c r="X59" s="271"/>
+      <c r="Y59" s="271"/>
+      <c r="Z59" s="271"/>
+      <c r="AA59" s="271"/>
       <c r="AB59" s="12">
         <f>VLOOKUP($Z$56,KEBDriveData[],4,FALSE)</f>
         <v>24</v>
@@ -15618,15 +15617,15 @@
         <v>16.5</v>
       </c>
       <c r="F60" s="153"/>
-      <c r="U60" s="269" t="s">
+      <c r="U60" s="271" t="s">
         <v>256</v>
       </c>
-      <c r="V60" s="269"/>
-      <c r="W60" s="269"/>
-      <c r="X60" s="269"/>
-      <c r="Y60" s="269"/>
-      <c r="Z60" s="269"/>
-      <c r="AA60" s="269"/>
+      <c r="V60" s="271"/>
+      <c r="W60" s="271"/>
+      <c r="X60" s="271"/>
+      <c r="Y60" s="271"/>
+      <c r="Z60" s="271"/>
+      <c r="AA60" s="271"/>
       <c r="AB60" s="12">
         <f>AB$59*VLOOKUP($Z$56,KEBDriveData[],5,FALSE)/100</f>
         <v>36</v>
@@ -15653,15 +15652,15 @@
         <f>$E$61/$E$66*380</f>
         <v>3535.1706172482595</v>
       </c>
-      <c r="U61" s="269" t="s">
+      <c r="U61" s="271" t="s">
         <v>231</v>
       </c>
-      <c r="V61" s="269"/>
-      <c r="W61" s="269"/>
-      <c r="X61" s="269"/>
-      <c r="Y61" s="269"/>
-      <c r="Z61" s="269"/>
-      <c r="AA61" s="269"/>
+      <c r="V61" s="271"/>
+      <c r="W61" s="271"/>
+      <c r="X61" s="271"/>
+      <c r="Y61" s="271"/>
+      <c r="Z61" s="271"/>
+      <c r="AA61" s="271"/>
       <c r="AB61" s="12">
         <f>AB$59*VLOOKUP($Z$56,KEBDriveData[],6,FALSE)/100</f>
         <v>43.2</v>
@@ -15685,10 +15684,10 @@
         <v>50</v>
       </c>
       <c r="F62" s="153"/>
-      <c r="AE62" s="278" t="s">
+      <c r="AE62" s="280" t="s">
         <v>241</v>
       </c>
-      <c r="AF62" s="278"/>
+      <c r="AF62" s="280"/>
     </row>
     <row r="63" spans="2:36" ht="15" x14ac:dyDescent="0.35">
       <c r="B63" s="154" t="s">
@@ -15703,15 +15702,15 @@
         <v>10.297778828128413</v>
       </c>
       <c r="F63" s="153"/>
-      <c r="U63" s="264" t="s">
+      <c r="U63" s="266" t="s">
         <v>257</v>
       </c>
-      <c r="V63" s="264"/>
-      <c r="W63" s="264"/>
-      <c r="X63" s="264"/>
-      <c r="Y63" s="264"/>
-      <c r="Z63" s="264"/>
-      <c r="AA63" s="264"/>
+      <c r="V63" s="266"/>
+      <c r="W63" s="266"/>
+      <c r="X63" s="266"/>
+      <c r="Y63" s="266"/>
+      <c r="Z63" s="266"/>
+      <c r="AA63" s="266"/>
       <c r="AB63" s="9">
         <f>AB$59*VLOOKUP($Z$56,KEBDriveData[],8,FALSE)/100</f>
         <v>0</v>
@@ -15740,15 +15739,15 @@
         <v>15.103999999999999</v>
       </c>
       <c r="F64" s="153"/>
-      <c r="U64" s="264" t="s">
+      <c r="U64" s="266" t="s">
         <v>258</v>
       </c>
-      <c r="V64" s="264"/>
-      <c r="W64" s="264"/>
-      <c r="X64" s="264"/>
-      <c r="Y64" s="264"/>
-      <c r="Z64" s="264"/>
-      <c r="AA64" s="264"/>
+      <c r="V64" s="266"/>
+      <c r="W64" s="266"/>
+      <c r="X64" s="266"/>
+      <c r="Y64" s="266"/>
+      <c r="Z64" s="266"/>
+      <c r="AA64" s="266"/>
       <c r="AB64" s="9">
         <f>AB$59*VLOOKUP($Z$56,KEBDriveData[],9,FALSE)/100</f>
         <v>21.12</v>
@@ -15777,15 +15776,15 @@
         <v>1.6022872772262502</v>
       </c>
       <c r="F65" s="153"/>
-      <c r="U65" s="264" t="s">
+      <c r="U65" s="266" t="s">
         <v>259</v>
       </c>
-      <c r="V65" s="264"/>
-      <c r="W65" s="264"/>
-      <c r="X65" s="264"/>
-      <c r="Y65" s="264"/>
-      <c r="Z65" s="264"/>
-      <c r="AA65" s="264"/>
+      <c r="V65" s="266"/>
+      <c r="W65" s="266"/>
+      <c r="X65" s="266"/>
+      <c r="Y65" s="266"/>
+      <c r="Z65" s="266"/>
+      <c r="AA65" s="266"/>
       <c r="AB65" s="9">
         <f>AB$59*VLOOKUP($Z$56,KEBDriveData[],10,FALSE)/100</f>
         <v>39.6</v>
@@ -15814,15 +15813,15 @@
         <v>322.47382755386337</v>
       </c>
       <c r="F66" s="153"/>
-      <c r="U66" s="264" t="s">
+      <c r="U66" s="266" t="s">
         <v>260</v>
       </c>
-      <c r="V66" s="264"/>
-      <c r="W66" s="264"/>
-      <c r="X66" s="264"/>
-      <c r="Y66" s="264"/>
-      <c r="Z66" s="264"/>
-      <c r="AA66" s="264"/>
+      <c r="V66" s="266"/>
+      <c r="W66" s="266"/>
+      <c r="X66" s="266"/>
+      <c r="Y66" s="266"/>
+      <c r="Z66" s="266"/>
+      <c r="AA66" s="266"/>
       <c r="AB66" s="9">
         <f>AB$59*VLOOKUP($Z$56,KEBDriveData[],11,FALSE)/100</f>
         <v>43.2</v>
@@ -15851,14 +15850,14 @@
         <v>16.600000000000001</v>
       </c>
       <c r="F67" s="158"/>
-      <c r="V67" s="265" t="s">
+      <c r="V67" s="267" t="s">
         <v>242</v>
       </c>
-      <c r="W67" s="265"/>
-      <c r="X67" s="265"/>
-      <c r="Y67" s="265"/>
-      <c r="Z67" s="265"/>
-      <c r="AA67" s="265"/>
+      <c r="W67" s="267"/>
+      <c r="X67" s="267"/>
+      <c r="Y67" s="267"/>
+      <c r="Z67" s="267"/>
+      <c r="AA67" s="267"/>
       <c r="AB67" s="73">
         <f>150/180</f>
         <v>0.83333333333333337</v>
@@ -15872,15 +15871,15 @@
       </c>
     </row>
     <row r="68" spans="2:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
-      <c r="U68" s="264" t="s">
+      <c r="U68" s="266" t="s">
         <v>261</v>
       </c>
-      <c r="V68" s="264"/>
-      <c r="W68" s="264"/>
-      <c r="X68" s="264"/>
-      <c r="Y68" s="264"/>
-      <c r="Z68" s="264"/>
-      <c r="AA68" s="264"/>
+      <c r="V68" s="266"/>
+      <c r="W68" s="266"/>
+      <c r="X68" s="266"/>
+      <c r="Y68" s="266"/>
+      <c r="Z68" s="266"/>
+      <c r="AA68" s="266"/>
       <c r="AB68" s="74">
         <f>MIN(AB63*$AB$67,$AB$61*$AB$67)</f>
         <v>0</v>
@@ -15891,15 +15890,15 @@
       <c r="AD68" s="61"/>
     </row>
     <row r="69" spans="2:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
-      <c r="U69" s="264" t="s">
+      <c r="U69" s="266" t="s">
         <v>262</v>
       </c>
-      <c r="V69" s="264"/>
-      <c r="W69" s="264"/>
-      <c r="X69" s="264"/>
-      <c r="Y69" s="264"/>
-      <c r="Z69" s="264"/>
-      <c r="AA69" s="264"/>
+      <c r="V69" s="266"/>
+      <c r="W69" s="266"/>
+      <c r="X69" s="266"/>
+      <c r="Y69" s="266"/>
+      <c r="Z69" s="266"/>
+      <c r="AA69" s="266"/>
       <c r="AB69" s="74">
         <f t="shared" ref="AB69:AB70" si="15">MIN(AB64*$AB$67,$AB$61*$AB$67)</f>
         <v>17.600000000000001</v>
@@ -15909,15 +15908,15 @@
       </c>
     </row>
     <row r="70" spans="2:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
-      <c r="U70" s="264" t="s">
+      <c r="U70" s="266" t="s">
         <v>263</v>
       </c>
-      <c r="V70" s="264"/>
-      <c r="W70" s="264"/>
-      <c r="X70" s="264"/>
-      <c r="Y70" s="264"/>
-      <c r="Z70" s="264"/>
-      <c r="AA70" s="264"/>
+      <c r="V70" s="266"/>
+      <c r="W70" s="266"/>
+      <c r="X70" s="266"/>
+      <c r="Y70" s="266"/>
+      <c r="Z70" s="266"/>
+      <c r="AA70" s="266"/>
       <c r="AB70" s="74">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -15928,15 +15927,15 @@
       <c r="AD70" s="15"/>
     </row>
     <row r="71" spans="2:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
-      <c r="U71" s="264" t="s">
+      <c r="U71" s="266" t="s">
         <v>264</v>
       </c>
-      <c r="V71" s="264"/>
-      <c r="W71" s="264"/>
-      <c r="X71" s="264"/>
-      <c r="Y71" s="264"/>
-      <c r="Z71" s="264"/>
-      <c r="AA71" s="264"/>
+      <c r="V71" s="266"/>
+      <c r="W71" s="266"/>
+      <c r="X71" s="266"/>
+      <c r="Y71" s="266"/>
+      <c r="Z71" s="266"/>
+      <c r="AA71" s="266"/>
       <c r="AB71" s="74">
         <f>MIN(AB66*$AB$67,$AB$61*$AB$67)</f>
         <v>36.000000000000007</v>
@@ -16132,11 +16131,11 @@
       <formula>$AC$47</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG46">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="AG45 AG48 AG50 AG52">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="num" val="1.05"/>
-        <cfvo type="num" val="1.25"/>
+        <cfvo type="percentile" val="1.5"/>
         <cfvo type="formula" val="$AC$67/100"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -16144,11 +16143,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG45 AG48 AG50 AG52">
-    <cfRule type="colorScale" priority="41">
+  <conditionalFormatting sqref="AG46">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="1.05"/>
-        <cfvo type="percentile" val="1.5"/>
+        <cfvo type="num" val="1.25"/>
         <cfvo type="formula" val="$AC$67/100"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -17470,17 +17469,17 @@
   <sheetData>
     <row r="1" spans="1:49" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="AC2" s="318" t="s">
+      <c r="AC2" s="320" t="s">
         <v>599</v>
       </c>
-      <c r="AD2" s="319"/>
-      <c r="AE2" s="319"/>
-      <c r="AF2" s="319"/>
-      <c r="AG2" s="319"/>
-      <c r="AH2" s="319"/>
-      <c r="AI2" s="319"/>
-      <c r="AJ2" s="319"/>
-      <c r="AK2" s="320"/>
+      <c r="AD2" s="321"/>
+      <c r="AE2" s="321"/>
+      <c r="AF2" s="321"/>
+      <c r="AG2" s="321"/>
+      <c r="AH2" s="321"/>
+      <c r="AI2" s="321"/>
+      <c r="AJ2" s="321"/>
+      <c r="AK2" s="322"/>
     </row>
     <row r="3" spans="1:49" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="56" t="s">
@@ -17494,18 +17493,18 @@
         <f>100*AE3/180</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="AC3" s="321" t="s">
+      <c r="AC3" s="323" t="s">
         <v>598</v>
       </c>
-      <c r="AD3" s="321"/>
+      <c r="AD3" s="323"/>
       <c r="AE3" s="228">
         <v>1.6</v>
       </c>
       <c r="AF3" s="118"/>
-      <c r="AG3" s="316" t="s">
+      <c r="AG3" s="318" t="s">
         <v>596</v>
       </c>
-      <c r="AH3" s="317"/>
+      <c r="AH3" s="319"/>
       <c r="AI3" s="225">
         <v>337.9</v>
       </c>
@@ -20332,130 +20331,130 @@
       </c>
       <c r="C1" s="110"/>
       <c r="D1" s="111"/>
-      <c r="E1" s="346" t="s">
+      <c r="E1" s="348" t="s">
         <v>396</v>
       </c>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
-      <c r="N1" s="347"/>
-      <c r="O1" s="347"/>
-      <c r="P1" s="347"/>
-      <c r="Q1" s="347"/>
-      <c r="R1" s="347"/>
-      <c r="S1" s="347"/>
-      <c r="T1" s="347"/>
-      <c r="U1" s="347"/>
-      <c r="V1" s="347"/>
-      <c r="W1" s="347"/>
-      <c r="X1" s="348"/>
-      <c r="Y1" s="346" t="s">
+      <c r="F1" s="349"/>
+      <c r="G1" s="349"/>
+      <c r="H1" s="349"/>
+      <c r="I1" s="349"/>
+      <c r="J1" s="349"/>
+      <c r="K1" s="349"/>
+      <c r="L1" s="349"/>
+      <c r="M1" s="349"/>
+      <c r="N1" s="349"/>
+      <c r="O1" s="349"/>
+      <c r="P1" s="349"/>
+      <c r="Q1" s="349"/>
+      <c r="R1" s="349"/>
+      <c r="S1" s="349"/>
+      <c r="T1" s="349"/>
+      <c r="U1" s="349"/>
+      <c r="V1" s="349"/>
+      <c r="W1" s="349"/>
+      <c r="X1" s="350"/>
+      <c r="Y1" s="348" t="s">
         <v>396</v>
       </c>
-      <c r="Z1" s="347"/>
-      <c r="AA1" s="347"/>
-      <c r="AB1" s="347"/>
-      <c r="AC1" s="347"/>
-      <c r="AD1" s="347"/>
-      <c r="AE1" s="347"/>
-      <c r="AF1" s="347"/>
-      <c r="AG1" s="347"/>
-      <c r="AH1" s="347"/>
-      <c r="AI1" s="347"/>
-      <c r="AJ1" s="347"/>
-      <c r="AK1" s="347"/>
-      <c r="AL1" s="347"/>
-      <c r="AM1" s="347"/>
-      <c r="AN1" s="347"/>
-      <c r="AO1" s="347"/>
-      <c r="AP1" s="347"/>
-      <c r="AQ1" s="347"/>
-      <c r="AR1" s="348"/>
-      <c r="AS1" s="346" t="s">
+      <c r="Z1" s="349"/>
+      <c r="AA1" s="349"/>
+      <c r="AB1" s="349"/>
+      <c r="AC1" s="349"/>
+      <c r="AD1" s="349"/>
+      <c r="AE1" s="349"/>
+      <c r="AF1" s="349"/>
+      <c r="AG1" s="349"/>
+      <c r="AH1" s="349"/>
+      <c r="AI1" s="349"/>
+      <c r="AJ1" s="349"/>
+      <c r="AK1" s="349"/>
+      <c r="AL1" s="349"/>
+      <c r="AM1" s="349"/>
+      <c r="AN1" s="349"/>
+      <c r="AO1" s="349"/>
+      <c r="AP1" s="349"/>
+      <c r="AQ1" s="349"/>
+      <c r="AR1" s="350"/>
+      <c r="AS1" s="348" t="s">
         <v>396</v>
       </c>
-      <c r="AT1" s="347"/>
-      <c r="AU1" s="347"/>
-      <c r="AV1" s="347"/>
-      <c r="AW1" s="347"/>
-      <c r="AX1" s="347"/>
-      <c r="AY1" s="347"/>
-      <c r="AZ1" s="347"/>
-      <c r="BA1" s="347"/>
-      <c r="BB1" s="347"/>
-      <c r="BC1" s="347"/>
-      <c r="BD1" s="347"/>
-      <c r="BE1" s="347"/>
-      <c r="BF1" s="347"/>
-      <c r="BG1" s="347"/>
-      <c r="BH1" s="347"/>
-      <c r="BI1" s="347"/>
-      <c r="BJ1" s="347"/>
-      <c r="BK1" s="347"/>
-      <c r="BL1" s="348"/>
-      <c r="BM1" s="334" t="s">
+      <c r="AT1" s="349"/>
+      <c r="AU1" s="349"/>
+      <c r="AV1" s="349"/>
+      <c r="AW1" s="349"/>
+      <c r="AX1" s="349"/>
+      <c r="AY1" s="349"/>
+      <c r="AZ1" s="349"/>
+      <c r="BA1" s="349"/>
+      <c r="BB1" s="349"/>
+      <c r="BC1" s="349"/>
+      <c r="BD1" s="349"/>
+      <c r="BE1" s="349"/>
+      <c r="BF1" s="349"/>
+      <c r="BG1" s="349"/>
+      <c r="BH1" s="349"/>
+      <c r="BI1" s="349"/>
+      <c r="BJ1" s="349"/>
+      <c r="BK1" s="349"/>
+      <c r="BL1" s="350"/>
+      <c r="BM1" s="336" t="s">
         <v>397</v>
       </c>
-      <c r="BN1" s="335"/>
-      <c r="BO1" s="335"/>
-      <c r="BP1" s="335"/>
-      <c r="BQ1" s="335"/>
-      <c r="BR1" s="335"/>
-      <c r="BS1" s="335"/>
-      <c r="BT1" s="335"/>
-      <c r="BU1" s="335"/>
-      <c r="BV1" s="335"/>
-      <c r="BW1" s="335"/>
-      <c r="BX1" s="335"/>
-      <c r="BY1" s="335"/>
-      <c r="BZ1" s="335"/>
-      <c r="CA1" s="335"/>
-      <c r="CB1" s="336"/>
+      <c r="BN1" s="337"/>
+      <c r="BO1" s="337"/>
+      <c r="BP1" s="337"/>
+      <c r="BQ1" s="337"/>
+      <c r="BR1" s="337"/>
+      <c r="BS1" s="337"/>
+      <c r="BT1" s="337"/>
+      <c r="BU1" s="337"/>
+      <c r="BV1" s="337"/>
+      <c r="BW1" s="337"/>
+      <c r="BX1" s="337"/>
+      <c r="BY1" s="337"/>
+      <c r="BZ1" s="337"/>
+      <c r="CA1" s="337"/>
+      <c r="CB1" s="338"/>
       <c r="CC1" s="207"/>
       <c r="CD1" s="207"/>
       <c r="CE1" s="207"/>
       <c r="CF1" s="207"/>
-      <c r="CG1" s="334" t="s">
+      <c r="CG1" s="336" t="s">
         <v>397</v>
       </c>
-      <c r="CH1" s="335"/>
-      <c r="CI1" s="335"/>
-      <c r="CJ1" s="335"/>
-      <c r="CK1" s="335"/>
-      <c r="CL1" s="335"/>
-      <c r="CM1" s="335"/>
-      <c r="CN1" s="335"/>
-      <c r="CO1" s="335"/>
-      <c r="CP1" s="335"/>
-      <c r="CQ1" s="335"/>
-      <c r="CR1" s="335"/>
-      <c r="CS1" s="335"/>
-      <c r="CT1" s="335"/>
-      <c r="CU1" s="335"/>
-      <c r="CV1" s="336"/>
-      <c r="CW1" s="334" t="s">
+      <c r="CH1" s="337"/>
+      <c r="CI1" s="337"/>
+      <c r="CJ1" s="337"/>
+      <c r="CK1" s="337"/>
+      <c r="CL1" s="337"/>
+      <c r="CM1" s="337"/>
+      <c r="CN1" s="337"/>
+      <c r="CO1" s="337"/>
+      <c r="CP1" s="337"/>
+      <c r="CQ1" s="337"/>
+      <c r="CR1" s="337"/>
+      <c r="CS1" s="337"/>
+      <c r="CT1" s="337"/>
+      <c r="CU1" s="337"/>
+      <c r="CV1" s="338"/>
+      <c r="CW1" s="336" t="s">
         <v>397</v>
       </c>
-      <c r="CX1" s="335"/>
-      <c r="CY1" s="335"/>
-      <c r="CZ1" s="335"/>
-      <c r="DA1" s="335"/>
-      <c r="DB1" s="335"/>
-      <c r="DC1" s="335"/>
-      <c r="DD1" s="335"/>
-      <c r="DE1" s="335"/>
-      <c r="DF1" s="335"/>
-      <c r="DG1" s="335"/>
-      <c r="DH1" s="335"/>
-      <c r="DI1" s="335"/>
-      <c r="DJ1" s="335"/>
-      <c r="DK1" s="335"/>
-      <c r="DL1" s="336"/>
+      <c r="CX1" s="337"/>
+      <c r="CY1" s="337"/>
+      <c r="CZ1" s="337"/>
+      <c r="DA1" s="337"/>
+      <c r="DB1" s="337"/>
+      <c r="DC1" s="337"/>
+      <c r="DD1" s="337"/>
+      <c r="DE1" s="337"/>
+      <c r="DF1" s="337"/>
+      <c r="DG1" s="337"/>
+      <c r="DH1" s="337"/>
+      <c r="DI1" s="337"/>
+      <c r="DJ1" s="337"/>
+      <c r="DK1" s="337"/>
+      <c r="DL1" s="338"/>
     </row>
     <row r="2" spans="2:116" s="109" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="110" t="s">
@@ -20463,154 +20462,154 @@
       </c>
       <c r="C2" s="110"/>
       <c r="D2" s="111"/>
-      <c r="E2" s="340" t="s">
+      <c r="E2" s="342" t="s">
         <v>398</v>
       </c>
-      <c r="F2" s="341"/>
-      <c r="G2" s="341"/>
-      <c r="H2" s="341"/>
-      <c r="I2" s="341"/>
-      <c r="J2" s="341"/>
-      <c r="K2" s="341"/>
-      <c r="L2" s="342"/>
-      <c r="M2" s="343" t="s">
+      <c r="F2" s="343"/>
+      <c r="G2" s="343"/>
+      <c r="H2" s="343"/>
+      <c r="I2" s="343"/>
+      <c r="J2" s="343"/>
+      <c r="K2" s="343"/>
+      <c r="L2" s="344"/>
+      <c r="M2" s="345" t="s">
         <v>399</v>
       </c>
-      <c r="N2" s="344"/>
-      <c r="O2" s="344"/>
-      <c r="P2" s="345"/>
-      <c r="Q2" s="337" t="s">
+      <c r="N2" s="346"/>
+      <c r="O2" s="346"/>
+      <c r="P2" s="347"/>
+      <c r="Q2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="R2" s="338"/>
-      <c r="S2" s="338"/>
-      <c r="T2" s="338"/>
-      <c r="U2" s="338"/>
-      <c r="V2" s="338"/>
-      <c r="W2" s="338"/>
-      <c r="X2" s="339"/>
-      <c r="Y2" s="340" t="s">
+      <c r="R2" s="340"/>
+      <c r="S2" s="340"/>
+      <c r="T2" s="340"/>
+      <c r="U2" s="340"/>
+      <c r="V2" s="340"/>
+      <c r="W2" s="340"/>
+      <c r="X2" s="341"/>
+      <c r="Y2" s="342" t="s">
         <v>398</v>
       </c>
-      <c r="Z2" s="341"/>
-      <c r="AA2" s="341"/>
-      <c r="AB2" s="341"/>
-      <c r="AC2" s="341"/>
-      <c r="AD2" s="341"/>
-      <c r="AE2" s="341"/>
-      <c r="AF2" s="342"/>
-      <c r="AG2" s="343" t="s">
+      <c r="Z2" s="343"/>
+      <c r="AA2" s="343"/>
+      <c r="AB2" s="343"/>
+      <c r="AC2" s="343"/>
+      <c r="AD2" s="343"/>
+      <c r="AE2" s="343"/>
+      <c r="AF2" s="344"/>
+      <c r="AG2" s="345" t="s">
         <v>399</v>
       </c>
-      <c r="AH2" s="344"/>
-      <c r="AI2" s="344"/>
-      <c r="AJ2" s="345"/>
-      <c r="AK2" s="337" t="s">
+      <c r="AH2" s="346"/>
+      <c r="AI2" s="346"/>
+      <c r="AJ2" s="347"/>
+      <c r="AK2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="AL2" s="338"/>
-      <c r="AM2" s="338"/>
-      <c r="AN2" s="338"/>
-      <c r="AO2" s="338"/>
-      <c r="AP2" s="338"/>
-      <c r="AQ2" s="338"/>
-      <c r="AR2" s="339"/>
-      <c r="AS2" s="340" t="s">
+      <c r="AL2" s="340"/>
+      <c r="AM2" s="340"/>
+      <c r="AN2" s="340"/>
+      <c r="AO2" s="340"/>
+      <c r="AP2" s="340"/>
+      <c r="AQ2" s="340"/>
+      <c r="AR2" s="341"/>
+      <c r="AS2" s="342" t="s">
         <v>398</v>
       </c>
-      <c r="AT2" s="341"/>
-      <c r="AU2" s="341"/>
-      <c r="AV2" s="341"/>
-      <c r="AW2" s="341"/>
-      <c r="AX2" s="341"/>
-      <c r="AY2" s="341"/>
-      <c r="AZ2" s="342"/>
-      <c r="BA2" s="344"/>
-      <c r="BB2" s="344"/>
-      <c r="BC2" s="344"/>
-      <c r="BD2" s="345"/>
-      <c r="BE2" s="337" t="s">
+      <c r="AT2" s="343"/>
+      <c r="AU2" s="343"/>
+      <c r="AV2" s="343"/>
+      <c r="AW2" s="343"/>
+      <c r="AX2" s="343"/>
+      <c r="AY2" s="343"/>
+      <c r="AZ2" s="344"/>
+      <c r="BA2" s="346"/>
+      <c r="BB2" s="346"/>
+      <c r="BC2" s="346"/>
+      <c r="BD2" s="347"/>
+      <c r="BE2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="BF2" s="338"/>
-      <c r="BG2" s="338"/>
-      <c r="BH2" s="338"/>
-      <c r="BI2" s="338"/>
-      <c r="BJ2" s="338"/>
-      <c r="BK2" s="338"/>
-      <c r="BL2" s="339"/>
-      <c r="BM2" s="340" t="s">
+      <c r="BF2" s="340"/>
+      <c r="BG2" s="340"/>
+      <c r="BH2" s="340"/>
+      <c r="BI2" s="340"/>
+      <c r="BJ2" s="340"/>
+      <c r="BK2" s="340"/>
+      <c r="BL2" s="341"/>
+      <c r="BM2" s="342" t="s">
         <v>398</v>
       </c>
-      <c r="BN2" s="341"/>
-      <c r="BO2" s="341"/>
-      <c r="BP2" s="341"/>
-      <c r="BQ2" s="341"/>
-      <c r="BR2" s="341"/>
-      <c r="BS2" s="341"/>
-      <c r="BT2" s="342"/>
-      <c r="BU2" s="343" t="s">
+      <c r="BN2" s="343"/>
+      <c r="BO2" s="343"/>
+      <c r="BP2" s="343"/>
+      <c r="BQ2" s="343"/>
+      <c r="BR2" s="343"/>
+      <c r="BS2" s="343"/>
+      <c r="BT2" s="344"/>
+      <c r="BU2" s="345" t="s">
         <v>399</v>
       </c>
-      <c r="BV2" s="344"/>
-      <c r="BW2" s="344"/>
-      <c r="BX2" s="345"/>
-      <c r="BY2" s="337" t="s">
+      <c r="BV2" s="346"/>
+      <c r="BW2" s="346"/>
+      <c r="BX2" s="347"/>
+      <c r="BY2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="BZ2" s="338"/>
-      <c r="CA2" s="338"/>
-      <c r="CB2" s="339"/>
-      <c r="CC2" s="337" t="s">
+      <c r="BZ2" s="340"/>
+      <c r="CA2" s="340"/>
+      <c r="CB2" s="341"/>
+      <c r="CC2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="CD2" s="338"/>
-      <c r="CE2" s="338"/>
-      <c r="CF2" s="339"/>
-      <c r="CG2" s="340" t="s">
+      <c r="CD2" s="340"/>
+      <c r="CE2" s="340"/>
+      <c r="CF2" s="341"/>
+      <c r="CG2" s="342" t="s">
         <v>398</v>
       </c>
-      <c r="CH2" s="341"/>
-      <c r="CI2" s="341"/>
-      <c r="CJ2" s="341"/>
-      <c r="CK2" s="341"/>
-      <c r="CL2" s="341"/>
-      <c r="CM2" s="341"/>
-      <c r="CN2" s="342"/>
-      <c r="CO2" s="343" t="s">
+      <c r="CH2" s="343"/>
+      <c r="CI2" s="343"/>
+      <c r="CJ2" s="343"/>
+      <c r="CK2" s="343"/>
+      <c r="CL2" s="343"/>
+      <c r="CM2" s="343"/>
+      <c r="CN2" s="344"/>
+      <c r="CO2" s="345" t="s">
         <v>399</v>
       </c>
-      <c r="CP2" s="344"/>
-      <c r="CQ2" s="344"/>
-      <c r="CR2" s="345"/>
-      <c r="CS2" s="337" t="s">
+      <c r="CP2" s="346"/>
+      <c r="CQ2" s="346"/>
+      <c r="CR2" s="347"/>
+      <c r="CS2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="CT2" s="338"/>
-      <c r="CU2" s="338"/>
-      <c r="CV2" s="339"/>
-      <c r="CW2" s="340" t="s">
+      <c r="CT2" s="340"/>
+      <c r="CU2" s="340"/>
+      <c r="CV2" s="341"/>
+      <c r="CW2" s="342" t="s">
         <v>398</v>
       </c>
-      <c r="CX2" s="341"/>
-      <c r="CY2" s="341"/>
-      <c r="CZ2" s="341"/>
-      <c r="DA2" s="341"/>
-      <c r="DB2" s="341"/>
-      <c r="DC2" s="341"/>
-      <c r="DD2" s="342"/>
-      <c r="DE2" s="343" t="s">
+      <c r="CX2" s="343"/>
+      <c r="CY2" s="343"/>
+      <c r="CZ2" s="343"/>
+      <c r="DA2" s="343"/>
+      <c r="DB2" s="343"/>
+      <c r="DC2" s="343"/>
+      <c r="DD2" s="344"/>
+      <c r="DE2" s="345" t="s">
         <v>399</v>
       </c>
-      <c r="DF2" s="344"/>
-      <c r="DG2" s="344"/>
-      <c r="DH2" s="345"/>
-      <c r="DI2" s="337" t="s">
+      <c r="DF2" s="346"/>
+      <c r="DG2" s="346"/>
+      <c r="DH2" s="347"/>
+      <c r="DI2" s="339" t="s">
         <v>400</v>
       </c>
-      <c r="DJ2" s="338"/>
-      <c r="DK2" s="338"/>
-      <c r="DL2" s="339"/>
+      <c r="DJ2" s="340"/>
+      <c r="DK2" s="340"/>
+      <c r="DL2" s="341"/>
     </row>
     <row r="3" spans="2:116" s="109" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="112" t="s">
@@ -20618,161 +20617,161 @@
       </c>
       <c r="C3" s="112"/>
       <c r="D3" s="113"/>
-      <c r="E3" s="322" t="s">
+      <c r="E3" s="324" t="s">
         <v>401</v>
       </c>
-      <c r="F3" s="323"/>
-      <c r="G3" s="323"/>
-      <c r="H3" s="323"/>
-      <c r="I3" s="323"/>
-      <c r="J3" s="323"/>
-      <c r="K3" s="323"/>
-      <c r="L3" s="324"/>
-      <c r="M3" s="322" t="s">
+      <c r="F3" s="325"/>
+      <c r="G3" s="325"/>
+      <c r="H3" s="325"/>
+      <c r="I3" s="325"/>
+      <c r="J3" s="325"/>
+      <c r="K3" s="325"/>
+      <c r="L3" s="326"/>
+      <c r="M3" s="324" t="s">
         <v>402</v>
       </c>
-      <c r="N3" s="323"/>
-      <c r="O3" s="323"/>
-      <c r="P3" s="324"/>
-      <c r="Q3" s="322" t="s">
+      <c r="N3" s="325"/>
+      <c r="O3" s="325"/>
+      <c r="P3" s="326"/>
+      <c r="Q3" s="324" t="s">
         <v>402</v>
       </c>
-      <c r="R3" s="323"/>
-      <c r="S3" s="323"/>
-      <c r="T3" s="323"/>
-      <c r="U3" s="323"/>
-      <c r="V3" s="323"/>
-      <c r="W3" s="323"/>
-      <c r="X3" s="324"/>
-      <c r="Y3" s="325" t="s">
+      <c r="R3" s="325"/>
+      <c r="S3" s="325"/>
+      <c r="T3" s="325"/>
+      <c r="U3" s="325"/>
+      <c r="V3" s="325"/>
+      <c r="W3" s="325"/>
+      <c r="X3" s="326"/>
+      <c r="Y3" s="327" t="s">
         <v>403</v>
       </c>
-      <c r="Z3" s="326"/>
-      <c r="AA3" s="326"/>
-      <c r="AB3" s="326"/>
-      <c r="AC3" s="326"/>
-      <c r="AD3" s="326"/>
-      <c r="AE3" s="326"/>
-      <c r="AF3" s="327"/>
-      <c r="AG3" s="325" t="s">
+      <c r="Z3" s="328"/>
+      <c r="AA3" s="328"/>
+      <c r="AB3" s="328"/>
+      <c r="AC3" s="328"/>
+      <c r="AD3" s="328"/>
+      <c r="AE3" s="328"/>
+      <c r="AF3" s="329"/>
+      <c r="AG3" s="327" t="s">
         <v>403</v>
       </c>
-      <c r="AH3" s="326"/>
-      <c r="AI3" s="326"/>
-      <c r="AJ3" s="327"/>
-      <c r="AK3" s="325" t="s">
+      <c r="AH3" s="328"/>
+      <c r="AI3" s="328"/>
+      <c r="AJ3" s="329"/>
+      <c r="AK3" s="327" t="s">
         <v>403</v>
       </c>
-      <c r="AL3" s="326"/>
-      <c r="AM3" s="326"/>
-      <c r="AN3" s="326"/>
-      <c r="AO3" s="326"/>
-      <c r="AP3" s="326"/>
-      <c r="AQ3" s="326"/>
-      <c r="AR3" s="327"/>
-      <c r="AS3" s="328" t="s">
+      <c r="AL3" s="328"/>
+      <c r="AM3" s="328"/>
+      <c r="AN3" s="328"/>
+      <c r="AO3" s="328"/>
+      <c r="AP3" s="328"/>
+      <c r="AQ3" s="328"/>
+      <c r="AR3" s="329"/>
+      <c r="AS3" s="330" t="s">
         <v>404</v>
       </c>
-      <c r="AT3" s="329"/>
-      <c r="AU3" s="329"/>
-      <c r="AV3" s="329"/>
-      <c r="AW3" s="329"/>
-      <c r="AX3" s="329"/>
-      <c r="AY3" s="329"/>
-      <c r="AZ3" s="330"/>
-      <c r="BA3" s="329"/>
-      <c r="BB3" s="329"/>
-      <c r="BC3" s="329"/>
-      <c r="BD3" s="330"/>
-      <c r="BE3" s="328" t="s">
+      <c r="AT3" s="331"/>
+      <c r="AU3" s="331"/>
+      <c r="AV3" s="331"/>
+      <c r="AW3" s="331"/>
+      <c r="AX3" s="331"/>
+      <c r="AY3" s="331"/>
+      <c r="AZ3" s="332"/>
+      <c r="BA3" s="331"/>
+      <c r="BB3" s="331"/>
+      <c r="BC3" s="331"/>
+      <c r="BD3" s="332"/>
+      <c r="BE3" s="330" t="s">
         <v>404</v>
       </c>
-      <c r="BF3" s="329"/>
-      <c r="BG3" s="329"/>
-      <c r="BH3" s="329"/>
-      <c r="BI3" s="329"/>
-      <c r="BJ3" s="329"/>
-      <c r="BK3" s="329"/>
-      <c r="BL3" s="330"/>
-      <c r="BM3" s="322" t="s">
+      <c r="BF3" s="331"/>
+      <c r="BG3" s="331"/>
+      <c r="BH3" s="331"/>
+      <c r="BI3" s="331"/>
+      <c r="BJ3" s="331"/>
+      <c r="BK3" s="331"/>
+      <c r="BL3" s="332"/>
+      <c r="BM3" s="324" t="s">
         <v>401</v>
       </c>
-      <c r="BN3" s="323"/>
-      <c r="BO3" s="323"/>
-      <c r="BP3" s="323"/>
-      <c r="BQ3" s="323"/>
-      <c r="BR3" s="323"/>
-      <c r="BS3" s="323"/>
-      <c r="BT3" s="324"/>
-      <c r="BU3" s="322" t="s">
+      <c r="BN3" s="325"/>
+      <c r="BO3" s="325"/>
+      <c r="BP3" s="325"/>
+      <c r="BQ3" s="325"/>
+      <c r="BR3" s="325"/>
+      <c r="BS3" s="325"/>
+      <c r="BT3" s="326"/>
+      <c r="BU3" s="324" t="s">
         <v>402</v>
       </c>
-      <c r="BV3" s="323"/>
-      <c r="BW3" s="323"/>
-      <c r="BX3" s="324"/>
-      <c r="BY3" s="322" t="s">
+      <c r="BV3" s="325"/>
+      <c r="BW3" s="325"/>
+      <c r="BX3" s="326"/>
+      <c r="BY3" s="324" t="s">
         <v>402</v>
       </c>
-      <c r="BZ3" s="323"/>
-      <c r="CA3" s="323"/>
-      <c r="CB3" s="324"/>
-      <c r="CC3" s="331" t="s">
+      <c r="BZ3" s="325"/>
+      <c r="CA3" s="325"/>
+      <c r="CB3" s="326"/>
+      <c r="CC3" s="333" t="s">
         <v>401</v>
       </c>
-      <c r="CD3" s="332"/>
-      <c r="CE3" s="332"/>
-      <c r="CF3" s="333"/>
-      <c r="CG3" s="325" t="s">
+      <c r="CD3" s="334"/>
+      <c r="CE3" s="334"/>
+      <c r="CF3" s="335"/>
+      <c r="CG3" s="327" t="s">
         <v>403</v>
       </c>
-      <c r="CH3" s="326"/>
-      <c r="CI3" s="326"/>
-      <c r="CJ3" s="326"/>
-      <c r="CK3" s="326"/>
-      <c r="CL3" s="326"/>
-      <c r="CM3" s="326"/>
-      <c r="CN3" s="327"/>
-      <c r="CO3" s="325" t="s">
+      <c r="CH3" s="328"/>
+      <c r="CI3" s="328"/>
+      <c r="CJ3" s="328"/>
+      <c r="CK3" s="328"/>
+      <c r="CL3" s="328"/>
+      <c r="CM3" s="328"/>
+      <c r="CN3" s="329"/>
+      <c r="CO3" s="327" t="s">
         <v>403</v>
       </c>
-      <c r="CP3" s="326"/>
-      <c r="CQ3" s="326"/>
-      <c r="CR3" s="327"/>
-      <c r="CS3" s="325" t="s">
+      <c r="CP3" s="328"/>
+      <c r="CQ3" s="328"/>
+      <c r="CR3" s="329"/>
+      <c r="CS3" s="327" t="s">
         <v>403</v>
       </c>
-      <c r="CT3" s="326"/>
-      <c r="CU3" s="326"/>
-      <c r="CV3" s="327"/>
-      <c r="CW3" s="328" t="s">
+      <c r="CT3" s="328"/>
+      <c r="CU3" s="328"/>
+      <c r="CV3" s="329"/>
+      <c r="CW3" s="330" t="s">
         <v>404</v>
       </c>
-      <c r="CX3" s="329"/>
-      <c r="CY3" s="329"/>
-      <c r="CZ3" s="329"/>
-      <c r="DA3" s="329"/>
-      <c r="DB3" s="329"/>
-      <c r="DC3" s="329"/>
-      <c r="DD3" s="330"/>
-      <c r="DE3" s="328" t="s">
+      <c r="CX3" s="331"/>
+      <c r="CY3" s="331"/>
+      <c r="CZ3" s="331"/>
+      <c r="DA3" s="331"/>
+      <c r="DB3" s="331"/>
+      <c r="DC3" s="331"/>
+      <c r="DD3" s="332"/>
+      <c r="DE3" s="330" t="s">
         <v>404</v>
       </c>
-      <c r="DF3" s="329"/>
-      <c r="DG3" s="329"/>
-      <c r="DH3" s="330"/>
-      <c r="DI3" s="328" t="s">
+      <c r="DF3" s="331"/>
+      <c r="DG3" s="331"/>
+      <c r="DH3" s="332"/>
+      <c r="DI3" s="330" t="s">
         <v>613</v>
       </c>
-      <c r="DJ3" s="329"/>
-      <c r="DK3" s="329"/>
-      <c r="DL3" s="330"/>
+      <c r="DJ3" s="331"/>
+      <c r="DK3" s="331"/>
+      <c r="DL3" s="332"/>
     </row>
     <row r="4" spans="2:116" x14ac:dyDescent="0.3">
-      <c r="B4" s="349" t="s">
+      <c r="B4" s="351" t="s">
         <v>318</v>
       </c>
-      <c r="C4" s="350"/>
-      <c r="D4" s="351"/>
+      <c r="C4" s="352"/>
+      <c r="D4" s="353"/>
       <c r="E4" s="107" t="s">
         <v>319</v>
       </c>
@@ -33414,10 +33413,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="352" t="s">
+      <c r="A1" s="354" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="352"/>
+      <c r="B1" s="354"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -36507,7 +36506,7 @@
   </sheetPr>
   <dimension ref="A1:V114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -36552,10 +36551,10 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="353" t="s">
+      <c r="A3" s="264" t="s">
         <v>623</v>
       </c>
-      <c r="B3" s="353" t="s">
+      <c r="B3" s="264" t="s">
         <v>319</v>
       </c>
       <c r="E3" t="s">
@@ -36688,7 +36687,7 @@
       <c r="L7" t="s">
         <v>725</v>
       </c>
-      <c r="M7" s="355" t="s">
+      <c r="M7" s="265" t="s">
         <v>729</v>
       </c>
     </row>
@@ -37259,10 +37258,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="353" t="s">
+      <c r="A27" s="264" t="s">
         <v>441</v>
       </c>
-      <c r="B27" s="354" t="s">
+      <c r="B27" s="265" t="s">
         <v>343</v>
       </c>
       <c r="E27" t="s">

</xml_diff>